<commit_message>
update to zimbabwe CCDR version (2023)
</commit_message>
<xml_diff>
--- a/Scenarios_to_compare.xlsx
+++ b/Scenarios_to_compare.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cowi-my.sharepoint.com/personal/rapy_cowi_com/Documents/WHAT_IF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAPY\OneDrive - COWI\Projects\IEc_Zimbabwe\WHAT_IF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F01FCFBF-04F5-4855-B944-57C587E472CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D7BA7EB5-35F8-42BF-BC53-9EBA2C2363F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED192D3-D26F-461F-9C76-36068DC4EB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="18" r:id="rId1"/>
-    <sheet name="ifpri" sheetId="19" r:id="rId2"/>
+    <sheet name="BAU" sheetId="23" r:id="rId1"/>
+    <sheet name="scenarios" sheetId="22" r:id="rId2"/>
+    <sheet name="fix" sheetId="24" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>SCENARIOS TO COMPARE</t>
   </si>
@@ -37,17 +47,200 @@
     <t>refscen</t>
   </si>
   <si>
-    <t>WHATIFmain</t>
-  </si>
-  <si>
-    <t>SSP2Xbase</t>
+    <t>BAU_observed</t>
+  </si>
+  <si>
+    <t>BAU_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>BAU_access-cm2</t>
+  </si>
+  <si>
+    <t>BAU_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>BAU_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>BAU_ec-earth3</t>
+  </si>
+  <si>
+    <t>BAU_fgoals-g3</t>
+  </si>
+  <si>
+    <t>BAUbtk_observed</t>
+  </si>
+  <si>
+    <t>BAUbtk_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>BAUbtk_access-cm2</t>
+  </si>
+  <si>
+    <t>BAUbtk_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>BAUbtk_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>BAUbtk_ec-earth3</t>
+  </si>
+  <si>
+    <t>BAUbtk_fgoals-g3</t>
+  </si>
+  <si>
+    <t>BAUwa_observed</t>
+  </si>
+  <si>
+    <t>BAUwa_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>BAUwa_access-cm2</t>
+  </si>
+  <si>
+    <t>BAUwa_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>BAUwa_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>BAUwa_ec-earth3</t>
+  </si>
+  <si>
+    <t>BAUwa_fgoals-g3</t>
+  </si>
+  <si>
+    <t>ASP_observed</t>
+  </si>
+  <si>
+    <t>ASP_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>ASP_access-cm2</t>
+  </si>
+  <si>
+    <t>ASP_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>ASP_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>ASP_ec-earth3</t>
+  </si>
+  <si>
+    <t>ASP_fgoals-g3</t>
+  </si>
+  <si>
+    <t>RES_observed</t>
+  </si>
+  <si>
+    <t>RES_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>RES_access-cm2</t>
+  </si>
+  <si>
+    <t>RES_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>RES_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>RES_ec-earth3</t>
+  </si>
+  <si>
+    <t>RES_fgoals-g3</t>
+  </si>
+  <si>
+    <t>BAUfix_observed</t>
+  </si>
+  <si>
+    <t>BAUfix_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>BAUfix_access-cm2</t>
+  </si>
+  <si>
+    <t>BAUfix_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>BAUfix_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>BAUfix_ec-earth3</t>
+  </si>
+  <si>
+    <t>BAUfix_fgoals-g3</t>
+  </si>
+  <si>
+    <t>BAUwafix_observed</t>
+  </si>
+  <si>
+    <t>BAUwafix_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>BAUwafix_access-cm2</t>
+  </si>
+  <si>
+    <t>BAUwafix_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>BAUwafix_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>BAUwafix_ec-earth3</t>
+  </si>
+  <si>
+    <t>BAUwafix_fgoals-g3</t>
+  </si>
+  <si>
+    <t>ASPfix_observed</t>
+  </si>
+  <si>
+    <t>ASPfix_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>ASPfix_access-cm2</t>
+  </si>
+  <si>
+    <t>ASPfix_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>ASPfix_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>ASPfix_ec-earth3</t>
+  </si>
+  <si>
+    <t>ASPfix_fgoals-g3</t>
+  </si>
+  <si>
+    <t>RESfix_observed</t>
+  </si>
+  <si>
+    <t>RESfix_mri-esm2-0</t>
+  </si>
+  <si>
+    <t>RESfix_access-cm2</t>
+  </si>
+  <si>
+    <t>RESfix_cnrm-esm2-1</t>
+  </si>
+  <si>
+    <t>RESfix_ec-earth3-veg</t>
+  </si>
+  <si>
+    <t>RESfix_ec-earth3</t>
+  </si>
+  <si>
+    <t>RESfix_fgoals-g3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,19 +268,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,10 +305,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,24 +594,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC778B4-C455-4BC3-83A5-43C86DD8C385}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EC340-D209-4DE0-BC06-AAB872143183}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -418,108 +619,78 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -527,21 +698,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D12169D-4F8A-4244-AB0B-EC74409C67A5}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CC25E1-9693-49E1-B661-16EB59D96933}">
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -549,18 +723,322 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68C8BED-F927-4B8D-BF91-27E6092BB628}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>